<commit_message>
fix upload file excel
</commit_message>
<xml_diff>
--- a/Format File Kata kabbar.xlsx
+++ b/Format File Kata kabbar.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Galangyp\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Galangyp\Desktop\SD Berkarakter Al Biruni\api\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0E9B7CD7-E2AE-4D02-9996-BF2BE83F1927}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55B25ABE-EB03-4D3C-9EC1-96FE4A42D627}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{073ACED2-BA58-447B-96B7-05675D08AB03}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -39,16 +39,16 @@
     <t>Indonesia</t>
   </si>
   <si>
-    <t>Aku</t>
-  </si>
-  <si>
-    <t>Kamu</t>
-  </si>
-  <si>
-    <t>Kita</t>
-  </si>
-  <si>
-    <t>Mereka</t>
+    <t>tes</t>
+  </si>
+  <si>
+    <t>set</t>
+  </si>
+  <si>
+    <t>tas</t>
+  </si>
+  <si>
+    <t>sat</t>
   </si>
 </sst>
 </file>

</xml_diff>